<commit_message>
Added Sci Rep rev
</commit_message>
<xml_diff>
--- a/ENG/data/service.xlsx
+++ b/ENG/data/service.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV-master\ENG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275DF182-81A7-4C8F-9C50-A24553D9D0B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A9D57C-6BFF-47CE-BE5B-D79DFA4AB95B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>what</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Evolution and Human Behavior</t>
+  </si>
+  <si>
+    <t>Scientific Reports</t>
   </si>
 </sst>
 </file>
@@ -962,17 +965,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1065,11 +1068,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,33 +1085,41 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added plos one to revs, youtube link for brazilian talk, and reorganised folders
</commit_message>
<xml_diff>
--- a/ENG/data/service.xlsx
+++ b/ENG/data/service.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV-master\ENG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCECDABF-4270-4D38-AC29-9A06DAAD3B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ECB687-4FBC-48B3-AF0A-7025CA8BD28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27870" yWindow="3465" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>what</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Edited by Juan David Leongomez, Katarzyna Pisanski, David Reby, Disa Sauter, Nadine Lavan, Marcus Perlman, &amp; Jaroslava Varella Valentova</t>
+  </si>
+  <si>
+    <t>PLOS ONE</t>
   </si>
 </sst>
 </file>
@@ -974,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,16 +1062,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1100,50 +1103,55 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>